<commit_message>
included ruben's change to add in the extra theoretical complexity chart
</commit_message>
<xml_diff>
--- a/experiments/speed/theo speed comparison.xlsx
+++ b/experiments/speed/theo speed comparison.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\experiments\speed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="18060" windowHeight="11640"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18060" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AlgorithmComplexityComparison" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="AllAlgorithmComplexityCompariso" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,14 +103,1611 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0989685284864001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1283741646848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1577798008832003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1871854370816002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.21659107328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2459967094783999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2754023456768002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3048079818751996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3342136180736004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3636192542720003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A360-4554-A9C6-A9043996444C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A360-4554-A9C6-A9043996444C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$15:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A360-4554-A9C6-A9043996444C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$15:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A360-4554-A9C6-A9043996444C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR-3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$15:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A360-4554-A9C6-A9043996444C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="92626944"/>
+        <c:axId val="92628864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="92626944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="0"/>
+                  <a:t> of pixels used as features</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU" sz="2000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92628864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="92628864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="0"/>
+                  <a:t>No. of operations  (x 10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="30000"/>
+                  <a:t>-9</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="0"/>
+                  <a:t> )</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92626944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0989685284864001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1283741646848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1577798008832003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1871854370816002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.21659107328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2459967094783999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2754023456768002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3048079818751996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3342136180736004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3636192542720003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$15:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$15:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR-3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$15:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$15:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28.668973809664003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.850234851328004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.031495892991998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.212756934655999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.394017976320001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.575279017984002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.756540059648003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.937801101312001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.119062142975999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.30032318464</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ICP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$15:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1218597.2926700094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9748778.0753662214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32902125.705117922</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77990223.538954362</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>152324654.93390486</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>263217003.24699873</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>417978851.83526528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>623921784.0557338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>888357383.26543331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1218597232.8213935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A77E-4D74-A426-48BDE70CD3FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84246528"/>
+        <c:axId val="84228352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84246528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="0"/>
+                  <a:t> of pixels used as features</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU" sz="2000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84228352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="84228352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000"/>
+                  <a:t>Approx</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="2000" baseline="0"/>
+                  <a:t>. No. of operations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84246528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -136,7 +1739,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -248,6 +1850,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9117-4C21-9DD6-ED741FD537F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -352,6 +1959,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9117-4C21-9DD6-ED741FD537F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -456,6 +2068,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9117-4C21-9DD6-ED741FD537F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -560,6 +2177,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9117-4C21-9DD6-ED741FD537F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -661,678 +2283,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="92626944"/>
-        <c:axId val="92628864"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="92626944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>%</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> of pixels used as features</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92628864"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="92628864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t>No. of operations  (x 10</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="30000"/>
-                  <a:t>-9</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> )</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92626944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Algorithm</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Complexity Comparison</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FM2D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="11"/>
-            <c:spPr>
-              <a:noFill/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$15:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0000000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000000000000006E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000015E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000019E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0000000000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$15:$E$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.0989685284864001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1283741646848</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1577798008832003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1871854370816002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.21659107328</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2459967094783999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2754023456768002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.3048079818751996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.3342136180736004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3636192542720003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PCA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="9"/>
-            <c:spPr>
-              <a:noFill/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$15:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0000000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000000000000006E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000015E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000019E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0000000000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$15:$G$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.4372109999999992E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FVR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="12"/>
-            <c:spPr>
-              <a:noFill/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$15:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0000000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000000000000006E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000015E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000019E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0000000000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$15:$I$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0367946758688658</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FFVR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$15:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0000000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000000000000006E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000015E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000019E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0000000000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$15:$J$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.24565563292581663</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$K$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FVR-3D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="15875"/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="plus"/>
-            <c:size val="10"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$15:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0000000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000000000000006E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000015E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000019E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0000000000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$K$15:$K$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0462318868688658</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9117-4C21-9DD6-ED741FD537F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1373,7 +2328,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1412,7 +2366,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1426,7 +2379,898 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Algorithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Complexity Comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0989685284864001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1283741646848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1577798008832003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1871854370816002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.21659107328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2459967094783999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2754023456768002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3048079818751996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3342136180736004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3636192542720003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4372109999999992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$15:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0367946758688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$15:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24565563292581663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FVR-3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$15:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0462318868688658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$15:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28.668973809664003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.850234851328004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.031495892991998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.212756934655999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.394017976320001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.575279017984002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.756540059648003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.937801101312001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.119062142975999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.30032318464</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ICP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000015E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000019E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$15:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1218597.2926700094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9748778.0753662214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32902125.705117922</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77990223.538954362</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>152324654.93390486</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>263217003.24699873</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>417978851.83526528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>623921784.0557338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>888357383.26543331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1218597232.8213935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-F012-4B67-84EE-3FED5D1CA2CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84246528"/>
+        <c:axId val="84228352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84246528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> of pixels used as features</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84228352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="84228352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Approx</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t>. No. of operations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84246528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1447,13 +3291,26 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{52F5B837-8917-4F96-9E26-B029F42CBD3C}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="65" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -1461,10 +3318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9279659" cy="6054148"/>
+    <xdr:ext cx="9302262" cy="6078415"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -1486,22 +3349,61 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308123" cy="6084277"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C982665-ADAB-4FB3-A7FF-E36819D7015F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>120096</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>135834</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>242016</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>39314</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>588064</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>130864</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>86360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1511,6 +3413,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>610208</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>47046</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C36B88C-27F4-4D26-BAA9-F6A5C4BC923E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1562,7 +3502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1595,9 +3535,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1630,6 +3587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1805,26 +3779,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="3" width="8.89453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.05078125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.05078125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.41796875" customWidth="1"/>
+    <col min="13" max="13" width="15.15625" customWidth="1"/>
+    <col min="14" max="14" width="18.83984375" customWidth="1"/>
+    <col min="15" max="15" width="16.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +3838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1024</v>
       </c>
@@ -1901,7 +3880,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1024</v>
       </c>
@@ -1944,7 +3923,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>1024</v>
       </c>
@@ -1987,7 +3966,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>1024</v>
       </c>
@@ -2030,7 +4009,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>1024</v>
       </c>
@@ -2073,7 +4052,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>1024</v>
       </c>
@@ -2116,7 +4095,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>1024</v>
       </c>
@@ -2159,7 +4138,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>1024</v>
       </c>
@@ -2202,7 +4181,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>1024</v>
       </c>
@@ -2245,7 +4224,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>1024</v>
       </c>
@@ -2288,7 +4267,7 @@
         <v>1046231886.8688657</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" t="s">
         <v>2</v>
       </c>
@@ -2314,347 +4293,347 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D15">
         <f>C2</f>
         <v>1E-4</v>
       </c>
       <c r="E15">
-        <f>E2/1000000000</f>
+        <f t="shared" ref="E15:K24" si="8">E2/1000000000</f>
         <v>2.0989685284864001</v>
       </c>
       <c r="F15">
-        <f>F2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>28.668973809664003</v>
       </c>
       <c r="G15">
-        <f>G2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H15">
-        <f>H2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1218597.2926700094</v>
       </c>
       <c r="I15">
-        <f>I2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J15">
-        <f>J2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K15">
-        <f>K2/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D16">
-        <f t="shared" ref="D16:D24" si="8">C3</f>
+        <f t="shared" ref="D16:D24" si="9">C3</f>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="E16">
-        <f>E3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.1283741646848</v>
       </c>
       <c r="F16">
-        <f>F3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>28.850234851328004</v>
       </c>
       <c r="G16">
-        <f>G3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H16">
-        <f>H3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9748778.0753662214</v>
       </c>
       <c r="I16">
-        <f>I3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J16">
-        <f>J3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K16">
-        <f>K3/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="E17">
-        <f>E4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.1577798008832003</v>
       </c>
       <c r="F17">
-        <f>F4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.031495892991998</v>
       </c>
       <c r="G17">
-        <f>G4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H17">
-        <f>H4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>32902125.705117922</v>
       </c>
       <c r="I17">
-        <f>I4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J17">
-        <f>J4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K17">
-        <f>K4/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="E18">
-        <f>E5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.1871854370816002</v>
       </c>
       <c r="F18">
-        <f>F5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.212756934655999</v>
       </c>
       <c r="G18">
-        <f>G5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H18">
-        <f>H5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>77990223.538954362</v>
       </c>
       <c r="I18">
-        <f>I5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J18">
-        <f>J5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K18">
-        <f>K5/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E19">
-        <f>E6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.21659107328</v>
       </c>
       <c r="F19">
-        <f>F6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.394017976320001</v>
       </c>
       <c r="G19">
-        <f>G6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H19">
-        <f>H6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>152324654.93390486</v>
       </c>
       <c r="I19">
-        <f>I6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J19">
-        <f>J6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K19">
-        <f>K6/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0000000000000006E-4</v>
       </c>
       <c r="E20">
-        <f>E7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.2459967094783999</v>
       </c>
       <c r="F20">
-        <f>F7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.575279017984002</v>
       </c>
       <c r="G20">
-        <f>G7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H20">
-        <f>H7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>263217003.24699873</v>
       </c>
       <c r="I20">
-        <f>I7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J20">
-        <f>J7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K20">
-        <f>K7/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.000000000000001E-4</v>
       </c>
       <c r="E21">
-        <f>E8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.2754023456768002</v>
       </c>
       <c r="F21">
-        <f>F8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.756540059648003</v>
       </c>
       <c r="G21">
-        <f>G8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H21">
-        <f>H8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>417978851.83526528</v>
       </c>
       <c r="I21">
-        <f>I8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J21">
-        <f>J8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K21">
-        <f>K8/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0000000000000015E-4</v>
       </c>
       <c r="E22">
-        <f>E9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.3048079818751996</v>
       </c>
       <c r="F22">
-        <f>F9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>29.937801101312001</v>
       </c>
       <c r="G22">
-        <f>G9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H22">
-        <f>H9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>623921784.0557338</v>
       </c>
       <c r="I22">
-        <f>I9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J22">
-        <f>J9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K22">
-        <f>K9/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.0000000000000019E-4</v>
       </c>
       <c r="E23">
-        <f>E10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.3342136180736004</v>
       </c>
       <c r="F23">
-        <f>F10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>30.119062142975999</v>
       </c>
       <c r="G23">
-        <f>G10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H23">
-        <f>H10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>888357383.26543331</v>
       </c>
       <c r="I23">
-        <f>I10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J23">
-        <f>J10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K23">
-        <f>K10/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0000000000000002E-3</v>
       </c>
       <c r="E24">
-        <f>E11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>2.3636192542720003</v>
       </c>
       <c r="F24">
-        <f>F11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>30.30032318464</v>
       </c>
       <c r="G24">
-        <f>G11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>9.4372109999999992E-3</v>
       </c>
       <c r="H24">
-        <f>H11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1218597232.8213935</v>
       </c>
       <c r="I24">
-        <f>I11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0367946758688658</v>
       </c>
       <c r="J24">
-        <f>J11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>0.24565563292581663</v>
       </c>
       <c r="K24">
-        <f>K11/1000000000</f>
+        <f t="shared" si="8"/>
         <v>1.0462318868688658</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="N26">
         <f>242/(640*480)</f>
         <v>7.8776041666666664E-4</v>
@@ -2667,24 +4646,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>